<commit_message>
loi chao mac dinh
</commit_message>
<xml_diff>
--- a/Backend/upload/knowledge_files/DSK_SU_KIEN_CHUNG.xlsx
+++ b/Backend/upload/knowledge_files/DSK_SU_KIEN_CHUNG.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TO NOI DUNG_THAO\CHATBOT\RAG 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7820CD-D938-4DE2-A323-B770A5314907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,12 +537,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;Ngày &quot;dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="&quot;Ngày &quot;dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -606,13 +607,6 @@
       <color rgb="FF0563C1"/>
       <name val="Times New Roman"/>
     </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -658,11 +652,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -733,7 +726,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -772,7 +765,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,12 +783,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1008,12 +997,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA836"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1021,7 +1010,7 @@
     <col min="1" max="1" width="4.21875" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="43.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="29.5546875" customWidth="1"/>
     <col min="6" max="6" width="21.21875" customWidth="1"/>
     <col min="7" max="7" width="26.5546875" customWidth="1"/>
@@ -1463,7 +1452,7 @@
       <c r="F11" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H11" s="12"/>
@@ -25774,26 +25763,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1"/>
-    <hyperlink ref="G12" r:id="rId2"/>
-    <hyperlink ref="G13" r:id="rId3"/>
-    <hyperlink ref="G20" r:id="rId4"/>
-    <hyperlink ref="G21" r:id="rId5"/>
-    <hyperlink ref="G22" r:id="rId6"/>
-    <hyperlink ref="G23" r:id="rId7"/>
-    <hyperlink ref="G24" r:id="rId8"/>
-    <hyperlink ref="G26" r:id="rId9"/>
-    <hyperlink ref="G27" r:id="rId10"/>
-    <hyperlink ref="G28" r:id="rId11"/>
-    <hyperlink ref="G29" r:id="rId12"/>
-    <hyperlink ref="G31" r:id="rId13"/>
-    <hyperlink ref="G32" r:id="rId14"/>
-    <hyperlink ref="G33" r:id="rId15"/>
-    <hyperlink ref="G34" r:id="rId16"/>
-    <hyperlink ref="G35" r:id="rId17"/>
-    <hyperlink ref="G39" r:id="rId18"/>
-    <hyperlink ref="G40" r:id="rId19"/>
-    <hyperlink ref="G11" r:id="rId20"/>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G23" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G27" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G28" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G29" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G31" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G32" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G33" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G34" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G35" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G39" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G40" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>